<commit_message>
Add Excel files and Python scripts for housing unit and common property house views
</commit_message>
<xml_diff>
--- a/H.xlsx
+++ b/H.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Project_A\Project_A\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0171CAF5-7E79-47CB-A963-9FEED2E2FF93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2064521-CF06-49DD-AF43-236C7158DF54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,22 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
-  <si>
-    <r>
-      <t>H</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>ID</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
   <si>
     <t>实际楼层</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -145,15 +130,15 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
+    <t>商业</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>其他</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
     <t>用途</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>商业</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>其他</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -214,7 +199,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -241,19 +226,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right/>
       <top style="thin">
         <color indexed="64"/>
@@ -270,7 +242,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -283,9 +255,6 @@
     <xf numFmtId="177" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="177" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -304,7 +273,7 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
@@ -591,306 +560,270 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="14.625" customWidth="1"/>
-    <col min="3" max="3" width="18.25" customWidth="1"/>
-    <col min="4" max="4" width="16.25" customWidth="1"/>
-    <col min="5" max="5" width="12.875" customWidth="1"/>
-    <col min="6" max="6" width="18.625" customWidth="1"/>
+    <col min="1" max="1" width="14.625" customWidth="1"/>
+    <col min="2" max="2" width="18.25" customWidth="1"/>
+    <col min="3" max="3" width="16.25" customWidth="1"/>
+    <col min="4" max="4" width="12.875" customWidth="1"/>
+    <col min="5" max="5" width="18.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
-        <v>1</v>
-      </c>
-      <c r="B2" s="7">
-        <v>1</v>
-      </c>
-      <c r="C2" s="10" t="s">
+      <c r="F1" s="11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="6">
+        <v>1</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="4">
+        <v>80.709999999999994</v>
+      </c>
+      <c r="D2" s="5">
+        <v>0</v>
+      </c>
+      <c r="E2" s="4">
+        <f t="shared" ref="E2:E11" si="0">D2+C2</f>
+        <v>80.709999999999994</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="6">
+        <v>1</v>
+      </c>
+      <c r="B3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="5">
-        <v>80.709999999999994</v>
-      </c>
-      <c r="E2" s="6">
-        <v>0</v>
-      </c>
-      <c r="F2" s="5">
-        <f t="shared" ref="F2:F11" si="0">E2+D2</f>
-        <v>80.709999999999994</v>
-      </c>
-      <c r="G2" s="12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="7">
-        <v>2</v>
-      </c>
-      <c r="B3" s="7">
-        <v>1</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>10</v>
+      <c r="C3" s="4">
+        <v>158.44</v>
       </c>
       <c r="D3" s="5">
-        <v>158.44</v>
-      </c>
-      <c r="E3" s="6">
-        <v>0</v>
-      </c>
-      <c r="F3" s="5">
+        <v>0</v>
+      </c>
+      <c r="E3" s="4">
         <f t="shared" si="0"/>
         <v>158.44</v>
       </c>
-      <c r="G3" s="12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="7">
-        <v>1</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>11</v>
+      <c r="F3" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="6">
+        <v>1</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="4">
+        <v>133.46</v>
       </c>
       <c r="D4" s="5">
-        <v>133.46</v>
-      </c>
-      <c r="E4" s="6">
-        <v>0</v>
-      </c>
-      <c r="F4" s="5">
+        <v>0</v>
+      </c>
+      <c r="E4" s="4">
         <f t="shared" si="0"/>
         <v>133.46</v>
       </c>
-      <c r="G4" s="12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="7">
-        <v>4</v>
-      </c>
-      <c r="B5" s="7">
-        <v>1</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>12</v>
+      <c r="F4" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
+        <v>1</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="4">
+        <v>109.58</v>
       </c>
       <c r="D5" s="5">
-        <v>109.58</v>
-      </c>
-      <c r="E5" s="6">
-        <v>0</v>
-      </c>
-      <c r="F5" s="5">
+        <v>0</v>
+      </c>
+      <c r="E5" s="4">
         <f t="shared" si="0"/>
         <v>109.58</v>
       </c>
-      <c r="G5" s="12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
-        <v>5</v>
-      </c>
-      <c r="B6" s="7">
-        <v>1</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>13</v>
+      <c r="F5" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="6">
+        <v>1</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="4">
+        <v>109.54</v>
       </c>
       <c r="D6" s="5">
-        <v>109.54</v>
-      </c>
-      <c r="E6" s="6">
-        <v>0</v>
-      </c>
-      <c r="F6" s="5">
+        <v>0</v>
+      </c>
+      <c r="E6" s="4">
         <f t="shared" si="0"/>
         <v>109.54</v>
       </c>
-      <c r="G6" s="12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="7">
-        <v>6</v>
-      </c>
-      <c r="B7" s="7">
-        <v>1</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>14</v>
+      <c r="F6" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
+        <v>1</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="4">
+        <v>144.88</v>
       </c>
       <c r="D7" s="5">
-        <v>144.88</v>
-      </c>
-      <c r="E7" s="6">
-        <v>0</v>
-      </c>
-      <c r="F7" s="5">
+        <v>0</v>
+      </c>
+      <c r="E7" s="4">
         <f t="shared" si="0"/>
         <v>144.88</v>
       </c>
-      <c r="G7" s="12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
-        <v>7</v>
-      </c>
-      <c r="B8" s="7">
-        <v>1</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>15</v>
+      <c r="F7" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
+        <v>1</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="4">
+        <v>85.09</v>
       </c>
       <c r="D8" s="5">
-        <v>85.09</v>
-      </c>
-      <c r="E8" s="6">
-        <v>0</v>
-      </c>
-      <c r="F8" s="5">
+        <v>0</v>
+      </c>
+      <c r="E8" s="4">
         <f t="shared" si="0"/>
         <v>85.09</v>
       </c>
-      <c r="G8" s="12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="7">
-        <v>8</v>
-      </c>
-      <c r="B9" s="7">
-        <v>1</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>16</v>
+      <c r="F8" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="6">
+        <v>1</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="4">
+        <v>83.99</v>
       </c>
       <c r="D9" s="5">
-        <v>83.99</v>
-      </c>
-      <c r="E9" s="6">
-        <v>0</v>
-      </c>
-      <c r="F9" s="5">
+        <v>0</v>
+      </c>
+      <c r="E9" s="4">
         <f t="shared" si="0"/>
         <v>83.99</v>
       </c>
-      <c r="G9" s="12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
-        <v>9</v>
-      </c>
-      <c r="B10" s="9">
+      <c r="F9" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="8">
         <v>2</v>
       </c>
-      <c r="C10" s="11" t="s">
-        <v>8</v>
+      <c r="B10" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="4">
+        <v>239.63</v>
       </c>
       <c r="D10" s="5">
-        <v>239.63</v>
-      </c>
-      <c r="E10" s="6">
-        <v>0</v>
-      </c>
-      <c r="F10" s="5">
+        <v>0</v>
+      </c>
+      <c r="E10" s="4">
         <f t="shared" si="0"/>
         <v>239.63</v>
       </c>
-      <c r="G10" s="12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="7">
-        <v>10</v>
-      </c>
-      <c r="B11" s="9">
+      <c r="F10" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="8">
         <v>2</v>
       </c>
-      <c r="C11" s="11" t="s">
-        <v>6</v>
+      <c r="B11" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="4">
+        <v>233.46</v>
       </c>
       <c r="D11" s="5">
-        <v>233.46</v>
-      </c>
-      <c r="E11" s="6">
         <v>7.56</v>
       </c>
-      <c r="F11" s="5">
+      <c r="E11" s="4">
         <f t="shared" si="0"/>
         <v>241.02</v>
       </c>
-      <c r="G11" s="12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="4">
-        <v>11</v>
-      </c>
-      <c r="B12" s="7">
-        <v>1</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>7</v>
+      <c r="F11" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="6">
+        <v>1</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="4">
+        <v>16.18</v>
       </c>
       <c r="D12" s="5">
+        <v>0</v>
+      </c>
+      <c r="E12" s="4">
+        <f>D12+C12</f>
         <v>16.18</v>
       </c>
-      <c r="E12" s="6">
-        <v>0</v>
-      </c>
-      <c r="F12" s="5">
-        <f>E12+D12</f>
-        <v>16.18</v>
-      </c>
-      <c r="G12" s="12" t="s">
-        <v>19</v>
+      <c r="F12" s="11" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>